<commit_message>
edit: remove unnecessary attributes
</commit_message>
<xml_diff>
--- a/artefacts/datadictionary/data_dictionary.xlsx
+++ b/artefacts/datadictionary/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Archives\ADS - Fatec\Semestre\04\LBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Archives\ADS - Fatec\Semestre\04\LBD\Projeto\gamestore\artefacts\datadictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D905BCCD-657F-44A9-B412-C02B210CF711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FEA52E-D95C-43E3-9A68-67C6CEAAD5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="928" xr2:uid="{C370E37D-0E0C-4CBA-B8BA-A6E603FB2DB6}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="585" firstSheet="10" activeTab="13" xr2:uid="{C370E37D-0E0C-4CBA-B8BA-A6E603FB2DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="FULL" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="117">
   <si>
     <t>Lista de Tabelas e Colunas Comentadas do Esquema GAMES</t>
   </si>
@@ -183,15 +183,6 @@
     <t>Nome da empresa desenvolvedora, não pode ser nula</t>
   </si>
   <si>
-    <t>DVD_SOBRE</t>
-  </si>
-  <si>
-    <t>Nvarchar2(1000)</t>
-  </si>
-  <si>
-    <t>Pequena descrição da empresa desenvolvedora, não pode ser nula</t>
-  </si>
-  <si>
     <t>Tabela DISTRIBUIDORAS: Tabela com dados das empresas distribuidoras, não pode ser nula</t>
   </si>
   <si>
@@ -199,12 +190,6 @@
   </si>
   <si>
     <t>Chave primária da tabela DISTRIBUIDORAS, não pode ser nula</t>
-  </si>
-  <si>
-    <t>DBR_SOBRE</t>
-  </si>
-  <si>
-    <t>Pequena descrição da empresa distribuidora, não pode ser nula</t>
   </si>
   <si>
     <t>DBR_NOME</t>
@@ -502,6 +487,13 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -511,17 +503,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2A3CB0-5BF9-4CBB-8DB2-E04B91D422AB}">
-  <dimension ref="B2:E98"/>
+  <dimension ref="B2:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:E11"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,92 +842,92 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1015,20 +1000,20 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -1073,20 +1058,20 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1131,20 +1116,20 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -1188,302 +1173,302 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+      <c r="B38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="11"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="C64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="11"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>9</v>
@@ -1497,243 +1482,243 @@
         <v>73</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="1" t="s">
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="C76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="11"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="1" t="s">
+      <c r="C82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="11"/>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="11"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="11"/>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="11"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
@@ -1741,7 +1726,7 @@
         <v>101</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>9</v>
@@ -1755,49 +1740,49 @@
         <v>103</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>9</v>
@@ -1811,21 +1796,21 @@
         <v>112</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>9</v>
@@ -1834,62 +1819,34 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B50:E50"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1912,20 +1869,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1995,20 +1952,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2063,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E8AF1B-AB39-4A6C-B873-E851069D2BD0}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,20 +2035,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2133,20 +2090,6 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2160,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10041ED7-88D3-40D0-A35E-B2FE86B540B1}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,20 +2118,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2206,7 +2149,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2215,35 +2158,21 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2259,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E266C7-E08A-475B-B97B-3F199E274400}">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,20 +2201,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2303,7 +2232,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2312,12 +2241,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>43</v>
@@ -2326,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2355,20 +2284,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2386,7 +2315,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2395,26 +2324,26 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -2423,40 +2352,40 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -2465,40 +2394,40 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
@@ -2507,7 +2436,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2536,20 +2465,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2567,7 +2496,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2576,12 +2505,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -2590,7 +2519,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2619,20 +2548,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2650,7 +2579,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2659,12 +2588,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -2673,7 +2602,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2702,20 +2631,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2733,7 +2662,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2742,12 +2671,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>43</v>
@@ -2756,40 +2685,40 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
@@ -2798,12 +2727,12 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -2812,12 +2741,12 @@
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -2826,12 +2755,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -2840,7 +2769,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2869,20 +2798,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2900,7 +2829,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -2909,12 +2838,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -2923,7 +2852,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2953,74 +2882,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3050,20 +2979,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -3081,7 +3010,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -3090,12 +3019,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>43</v>
@@ -3104,7 +3033,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3133,20 +3062,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -3219,7 +3148,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="7"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
edit: added new column
</commit_message>
<xml_diff>
--- a/artefacts/datadictionary/data_dictionary.xlsx
+++ b/artefacts/datadictionary/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Archives\ADS - Fatec\Semestre\04\LBD\Projeto\gamestore\artefacts\datadictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FEA52E-D95C-43E3-9A68-67C6CEAAD5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E04F98-0C2C-40B4-92D7-83C3D3006354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="585" firstSheet="10" activeTab="13" xr2:uid="{C370E37D-0E0C-4CBA-B8BA-A6E603FB2DB6}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="585" xr2:uid="{C370E37D-0E0C-4CBA-B8BA-A6E603FB2DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="FULL" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="118">
   <si>
     <t>Lista de Tabelas e Colunas Comentadas do Esquema GAMES</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>Data que de cadastro so usuário, não pode ser nula</t>
+  </si>
+  <si>
+    <t>ITC_CMP_DATA</t>
   </si>
 </sst>
 </file>
@@ -484,16 +487,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -503,6 +504,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -821,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2A3CB0-5BF9-4CBB-8DB2-E04B91D422AB}">
-  <dimension ref="B2:E96"/>
+  <dimension ref="B2:E97"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,20 +846,20 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -914,20 +918,20 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1000,20 +1004,20 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -1058,20 +1062,20 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1115,738 +1119,752 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="6"/>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="10"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="6"/>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="1" t="s">
+      <c r="D97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B50:E50"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1869,20 +1887,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1937,10 +1955,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A71F91B-756E-4107-BCEC-6241401C7F6D}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,20 +1970,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2006,6 +2024,20 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2035,20 +2067,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2118,20 +2150,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2188,7 +2220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E266C7-E08A-475B-B97B-3F199E274400}">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2201,20 +2233,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2284,20 +2316,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2465,20 +2497,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2548,20 +2580,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2631,20 +2663,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2798,20 +2830,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -2882,20 +2914,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2979,20 +3011,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -3062,20 +3094,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">

</xml_diff>

<commit_message>
Update fields from tables on data dictionary
</commit_message>
<xml_diff>
--- a/artefacts/datadictionary/data_dictionary.xlsx
+++ b/artefacts/datadictionary/data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Archives\ADS - Fatec\Semestre\04\LBD\Projeto\gamestore\artefacts\datadictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E04F98-0C2C-40B4-92D7-83C3D3006354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54B9108-113F-4D62-B575-1DA478081675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="585" xr2:uid="{C370E37D-0E0C-4CBA-B8BA-A6E603FB2DB6}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="120">
   <si>
     <t>Lista de Tabelas e Colunas Comentadas do Esquema GAMES</t>
   </si>
@@ -105,24 +105,15 @@
     <t>CMP_USU_ID</t>
   </si>
   <si>
-    <t>Chave primária da tabela COMPRAS, uma chave estrangeira que vem da tabela USUARIOS</t>
-  </si>
-  <si>
     <t>CMP_FPG_ID</t>
   </si>
   <si>
-    <t>Chave primária da tabela COMPRAS, uma chave estrangeira que vem da tabela FORMAS_DE_PAGAMENTO</t>
-  </si>
-  <si>
     <t>CMP_DATA</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Data em que a compra foi realizada</t>
-  </si>
-  <si>
     <t>CMP_VALOR_TOTAL</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>Chave primária da tabela ITENS_DE_COMPRA, uma chave estrangeira que vem da tabela JOGOS, não pode ser nula</t>
   </si>
   <si>
-    <t>ITC_CMP_USU_ID</t>
-  </si>
-  <si>
     <t>Chave primária da tabela ITENS_DE_COMPRA, uma chave estrangeira que vem da tabela COMPRAS, não pode ser nula</t>
   </si>
   <si>
@@ -396,17 +384,35 @@
     <t>USU_DATA_CRIACAO</t>
   </si>
   <si>
-    <t>Data que de cadastro so usuário, não pode ser nula</t>
-  </si>
-  <si>
-    <t>ITC_CMP_DATA</t>
+    <t>CMP_ID</t>
+  </si>
+  <si>
+    <t>Chave primária da tabela COMPRAS</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que vem da tabela USUARIOS</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que vem da tabela FORMAS_DE_PAGAMENTO</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>Data e hora em que a compra foi realizada</t>
+  </si>
+  <si>
+    <t>ITC_CMP_ID</t>
+  </si>
+  <si>
+    <t>Data de cadastro do usuário, não pode ser nula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,13 +420,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -487,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -495,22 +523,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,51 +873,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2A3CB0-5BF9-4CBB-8DB2-E04B91D422AB}">
   <dimension ref="B2:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -918,52 +964,52 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>19</v>
+      <c r="B14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -972,142 +1018,142 @@
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="14" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="14" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>8</v>
@@ -1116,56 +1162,56 @@
         <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>38</v>
+      <c r="B30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="B32" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
@@ -1174,56 +1220,56 @@
         <v>9</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="10"/>
+      <c r="B38" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
@@ -1232,56 +1278,56 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
+      <c r="B44" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="10"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
@@ -1290,56 +1336,56 @@
         <v>9</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="10"/>
+      <c r="B50" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="17"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>8</v>
@@ -1348,56 +1394,56 @@
         <v>9</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="10"/>
+      <c r="B56" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="17"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>8</v>
@@ -1406,12 +1452,12 @@
         <v>9</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>8</v>
@@ -1420,42 +1466,42 @@
         <v>9</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
+      <c r="B62" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="17"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="10"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="20"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
@@ -1464,82 +1510,82 @@
         <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>8</v>
@@ -1548,12 +1594,12 @@
         <v>9</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>8</v>
@@ -1562,42 +1608,42 @@
         <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="10"/>
+      <c r="B74" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="10"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="20"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
@@ -1606,12 +1652,12 @@
         <v>9</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
@@ -1620,42 +1666,42 @@
         <v>9</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="10"/>
+      <c r="B80" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="10"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="20"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>8</v>
@@ -1664,12 +1710,12 @@
         <v>9</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>8</v>
@@ -1678,42 +1724,42 @@
         <v>9</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="10"/>
+      <c r="B86" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="17"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="10"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="20"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>8</v>
@@ -1722,123 +1768,139 @@
         <v>9</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B50:E50"/>
     <mergeCell ref="B80:E80"/>
     <mergeCell ref="B81:E81"/>
     <mergeCell ref="B86:E86"/>
@@ -1849,24 +1911,9 @@
     <mergeCell ref="B63:E63"/>
     <mergeCell ref="B74:E74"/>
     <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B50:E50"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1875,7 +1922,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,61 +1934,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1955,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A71F91B-756E-4107-BCEC-6241401C7F6D}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,75 +2017,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2088,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,61 +2100,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2138,7 +2171,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,61 +2183,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2254,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,61 +2266,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2304,7 +2337,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,159 +2349,159 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>116</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2485,7 +2518,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,61 +2530,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2580,61 +2613,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2651,7 +2684,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B2" sqref="B2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,145 +2696,145 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2818,7 +2851,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,61 +2863,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2934,7 @@
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B2" sqref="B2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,74 +2947,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2999,7 +3032,7 @@
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,61 +3044,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3082,7 +3115,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B2" sqref="B2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,89 +3127,103 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>